<commit_message>
update excel nota invoice
</commit_message>
<xml_diff>
--- a/kerjaan/cuti-msj/tambahan/tawaran biaya modul tiket.xlsx
+++ b/kerjaan/cuti-msj/tambahan/tawaran biaya modul tiket.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1B9878-5139-4BA0-9D13-B07FADEA8D76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80877D35-29FC-48EA-B5D3-5B1EC69521A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Jasa Perbaikan Website</t>
   </si>
   <si>
-    <t>wa: 0815 4514 3654 | web: zenzen.web.id</t>
-  </si>
-  <si>
     <t>Uraian</t>
   </si>
   <si>
@@ -47,6 +44,21 @@
   </si>
   <si>
     <t>hari</t>
+  </si>
+  <si>
+    <t>web: gg.gg/jasazen</t>
+  </si>
+  <si>
+    <t>Tanggal Pembayaran</t>
+  </si>
+  <si>
+    <t>Banyaknya</t>
+  </si>
+  <si>
+    <t>Sisa</t>
+  </si>
+  <si>
+    <t>24 Agustus 2023</t>
   </si>
 </sst>
 </file>
@@ -121,26 +133,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,92 +441,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <f>B5*150000</f>
         <v>300000</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
         <v>50000</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <f>D5-E5</f>
         <v>250000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="4">
         <f>F5</f>
         <v>250000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3">
+        <v>250000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>